<commit_message>
Rerun model with Eigenvalues as ref
</commit_message>
<xml_diff>
--- a/ml_scripts/Final.xlsx
+++ b/ml_scripts/Final.xlsx
@@ -538,10 +538,10 @@
         <v>8488</v>
       </c>
       <c r="M2" t="n">
-        <v>2.519866825084559</v>
+        <v>2.726540799331899</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.6091174611646316</v>
+        <v>-0.6011343761358734</v>
       </c>
     </row>
     <row r="3">
@@ -582,10 +582,10 @@
         <v>8399</v>
       </c>
       <c r="M3" t="n">
-        <v>1.786566202187576</v>
+        <v>2.016045188666966</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.6379245869445547</v>
+        <v>-0.6345055137861857</v>
       </c>
     </row>
     <row r="4">
@@ -626,10 +626,10 @@
         <v>8328</v>
       </c>
       <c r="M4" t="n">
-        <v>2.328681464543676</v>
+        <v>2.482827041370223</v>
       </c>
       <c r="N4" t="n">
-        <v>0.4321269067828439</v>
+        <v>0.4403078241362656</v>
       </c>
     </row>
     <row r="5">
@@ -670,10 +670,10 @@
         <v>8306</v>
       </c>
       <c r="M5" t="n">
-        <v>1.733256691471264</v>
+        <v>1.937743539785606</v>
       </c>
       <c r="N5" t="n">
-        <v>-2.308492417863555</v>
+        <v>-2.304290298803274</v>
       </c>
     </row>
     <row r="6">
@@ -714,10 +714,10 @@
         <v>8286</v>
       </c>
       <c r="M6" t="n">
-        <v>2.236244875579776</v>
+        <v>2.380447653508261</v>
       </c>
       <c r="N6" t="n">
-        <v>-1.548488814448006</v>
+        <v>-1.540343857027132</v>
       </c>
     </row>
     <row r="7">
@@ -758,10 +758,10 @@
         <v>8272</v>
       </c>
       <c r="M7" t="n">
-        <v>1.585253374053913</v>
+        <v>1.743798000363266</v>
       </c>
       <c r="N7" t="n">
-        <v>0.7466407170545297</v>
+        <v>0.7509337052057601</v>
       </c>
     </row>
     <row r="8">
@@ -802,10 +802,10 @@
         <v>8216</v>
       </c>
       <c r="M8" t="n">
-        <v>1.547782002225483</v>
+        <v>1.69804703729039</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.5113466503073231</v>
+        <v>-0.5071567395949607</v>
       </c>
     </row>
     <row r="9">
@@ -846,10 +846,10 @@
         <v>8189</v>
       </c>
       <c r="M9" t="n">
-        <v>1.347818947128424</v>
+        <v>1.51113383848651</v>
       </c>
       <c r="N9" t="n">
-        <v>0.08919156615478192</v>
+        <v>0.09182366035968278</v>
       </c>
     </row>
     <row r="10">
@@ -890,10 +890,10 @@
         <v>8180</v>
       </c>
       <c r="M10" t="n">
-        <v>1.65111327372477</v>
+        <v>1.766247821525466</v>
       </c>
       <c r="N10" t="n">
-        <v>1.249776656812605</v>
+        <v>1.255427573142105</v>
       </c>
     </row>
     <row r="11">
@@ -934,10 +934,10 @@
         <v>8167</v>
       </c>
       <c r="M11" t="n">
-        <v>1.745288678233408</v>
+        <v>1.832616256344844</v>
       </c>
       <c r="N11" t="n">
-        <v>1.212600779450678</v>
+        <v>1.219471586030356</v>
       </c>
     </row>
     <row r="12">
@@ -978,10 +978,10 @@
         <v>8143</v>
       </c>
       <c r="M12" t="n">
-        <v>0.9542707045750156</v>
+        <v>1.109896023217602</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.5068444892259416</v>
+        <v>-0.5060339354598691</v>
       </c>
     </row>
     <row r="13">
@@ -1022,10 +1022,10 @@
         <v>8114</v>
       </c>
       <c r="M13" t="n">
-        <v>0.97801809025797</v>
+        <v>1.117460487216756</v>
       </c>
       <c r="N13" t="n">
-        <v>-1.992282418143098</v>
+        <v>-1.990620319607662</v>
       </c>
     </row>
     <row r="14">
@@ -1066,10 +1066,10 @@
         <v>8093</v>
       </c>
       <c r="M14" t="n">
-        <v>1.383526088504179</v>
+        <v>1.47380944131921</v>
       </c>
       <c r="N14" t="n">
-        <v>-0.8335356428966431</v>
+        <v>-0.8287384980605181</v>
       </c>
     </row>
     <row r="15">
@@ -1110,10 +1110,10 @@
         <v>8083</v>
       </c>
       <c r="M15" t="n">
-        <v>0.8539660627507778</v>
+        <v>0.9601669596683547</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.4564055665366182</v>
+        <v>-0.4547794531366097</v>
       </c>
     </row>
     <row r="16">
@@ -1154,10 +1154,10 @@
         <v>8036</v>
       </c>
       <c r="M16" t="n">
-        <v>0.7551151323577663</v>
+        <v>0.8569969943998081</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.03792183767379333</v>
+        <v>-0.03661183848374457</v>
       </c>
     </row>
     <row r="17">
@@ -1198,10 +1198,10 @@
         <v>8021</v>
       </c>
       <c r="M17" t="n">
-        <v>0.007497411545973695</v>
+        <v>0.06179640846755643</v>
       </c>
       <c r="N17" t="n">
-        <v>4.423673285736633</v>
+        <v>4.421600526028747</v>
       </c>
     </row>
     <row r="18">
@@ -1242,10 +1242,10 @@
         <v>7869</v>
       </c>
       <c r="M18" t="n">
-        <v>0.4359233833550684</v>
+        <v>0.4477960896050738</v>
       </c>
       <c r="N18" t="n">
-        <v>2.130731853000662</v>
+        <v>2.132266818982213</v>
       </c>
     </row>
     <row r="19">
@@ -1286,10 +1286,10 @@
         <v>7860</v>
       </c>
       <c r="M19" t="n">
-        <v>-0.0974995682636883</v>
+        <v>-0.03471211841238647</v>
       </c>
       <c r="N19" t="n">
-        <v>-1.820993931869887</v>
+        <v>-1.822425721826589</v>
       </c>
     </row>
     <row r="20">
@@ -1330,10 +1330,10 @@
         <v>7859</v>
       </c>
       <c r="M20" t="n">
-        <v>0.5849306780903817</v>
+        <v>0.5242369474050622</v>
       </c>
       <c r="N20" t="n">
-        <v>0.9857886595975351</v>
+        <v>0.9902466754491056</v>
       </c>
     </row>
     <row r="21">
@@ -1374,10 +1374,10 @@
         <v>7781</v>
       </c>
       <c r="M21" t="n">
-        <v>-0.5137046534479132</v>
+        <v>-0.4803275668441702</v>
       </c>
       <c r="N21" t="n">
-        <v>0.126982448908762</v>
+        <v>0.1231207365779711</v>
       </c>
     </row>
     <row r="22">
@@ -1418,10 +1418,10 @@
         <v>7753</v>
       </c>
       <c r="M22" t="n">
-        <v>-0.6588365909555421</v>
+        <v>-0.6176040000585149</v>
       </c>
       <c r="N22" t="n">
-        <v>-0.01459209035897613</v>
+        <v>-0.01932303281527617</v>
       </c>
     </row>
     <row r="23">
@@ -1462,10 +1462,10 @@
         <v>7745</v>
       </c>
       <c r="M23" t="n">
-        <v>-0.220637306946247</v>
+        <v>-0.2281719767641495</v>
       </c>
       <c r="N23" t="n">
-        <v>0.6217375539366373</v>
+        <v>0.6206050253861982</v>
       </c>
     </row>
     <row r="24">
@@ -1506,10 +1506,10 @@
         <v>7743</v>
       </c>
       <c r="M24" t="n">
-        <v>-0.7256291517063368</v>
+        <v>-0.768397556496339</v>
       </c>
       <c r="N24" t="n">
-        <v>-0.2222625795985106</v>
+        <v>-0.2251153793747109</v>
       </c>
     </row>
     <row r="25">
@@ -1550,10 +1550,10 @@
         <v>7623</v>
       </c>
       <c r="M25" t="n">
-        <v>-0.3380875484230835</v>
+        <v>-0.4555226062042685</v>
       </c>
       <c r="N25" t="n">
-        <v>-0.604277789031906</v>
+        <v>-0.602867727774186</v>
       </c>
     </row>
     <row r="26">
@@ -1594,10 +1594,10 @@
         <v>7579</v>
       </c>
       <c r="M26" t="n">
-        <v>-1.066344372373605</v>
+        <v>-1.151055804845307</v>
       </c>
       <c r="N26" t="n">
-        <v>-1.518084777823786</v>
+        <v>-1.5214252792935</v>
       </c>
     </row>
     <row r="27">
@@ -1638,10 +1638,10 @@
         <v>7517</v>
       </c>
       <c r="M27" t="n">
-        <v>-1.028001741545042</v>
+        <v>-1.13268492108448</v>
       </c>
       <c r="N27" t="n">
-        <v>-1.977810433852048</v>
+        <v>-1.979855779964381</v>
       </c>
     </row>
     <row r="28">
@@ -1682,10 +1682,10 @@
         <v>7505</v>
       </c>
       <c r="M28" t="n">
-        <v>-1.044459346481627</v>
+        <v>-1.216094983469689</v>
       </c>
       <c r="N28" t="n">
-        <v>2.365286930918008</v>
+        <v>2.364078146885753</v>
       </c>
     </row>
     <row r="29">
@@ -1726,10 +1726,10 @@
         <v>7422</v>
       </c>
       <c r="M29" t="n">
-        <v>-1.575338007460825</v>
+        <v>-1.766923878431851</v>
       </c>
       <c r="N29" t="n">
-        <v>-1.410620842627701</v>
+        <v>-1.413642542745665</v>
       </c>
     </row>
     <row r="30">
@@ -1770,10 +1770,10 @@
         <v>7310</v>
       </c>
       <c r="M30" t="n">
-        <v>-1.685301756593662</v>
+        <v>-1.92785212602099</v>
       </c>
       <c r="N30" t="n">
-        <v>0.525386876267541</v>
+        <v>0.5230262448985582</v>
       </c>
     </row>
     <row r="31">
@@ -1814,10 +1814,10 @@
         <v>7237</v>
       </c>
       <c r="M31" t="n">
-        <v>-2.151116236500298</v>
+        <v>-2.355787045532871</v>
       </c>
       <c r="N31" t="n">
-        <v>2.639922822697948</v>
+        <v>2.633818040410711</v>
       </c>
     </row>
     <row r="32">
@@ -1858,10 +1858,10 @@
         <v>7231</v>
       </c>
       <c r="M32" t="n">
-        <v>-2.502339080144659</v>
+        <v>-2.824925024395875</v>
       </c>
       <c r="N32" t="n">
-        <v>0.7136264615723602</v>
+        <v>0.708853052214381</v>
       </c>
     </row>
     <row r="33">
@@ -1902,10 +1902,10 @@
         <v>7016</v>
       </c>
       <c r="M33" t="n">
-        <v>-3.447281748873429</v>
+        <v>-3.749062012438849</v>
       </c>
       <c r="N33" t="n">
-        <v>-1.235390683890309</v>
+        <v>-1.245588494951435</v>
       </c>
     </row>
     <row r="34">
@@ -1946,10 +1946,10 @@
         <v>6907</v>
       </c>
       <c r="M34" t="n">
-        <v>-9.593965550106963</v>
+        <v>-10.46091115623349</v>
       </c>
       <c r="N34" t="n">
-        <v>-0.6165764301623999</v>
+        <v>-0.6436418939369377</v>
       </c>
     </row>
     <row r="35">
@@ -2008,10 +2008,10 @@
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="n">
-        <v>2.21342277415294</v>
+        <v>2.522426249260381</v>
       </c>
       <c r="N36" t="n">
-        <v>0.5994959255281623</v>
+        <v>0.6025210670707041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>